<commit_message>
update dados t18.1 e t18.2
</commit_message>
<xml_diff>
--- a/Data/t18.1.xlsx
+++ b/Data/t18.1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E217"/>
+  <dimension ref="A1:E235"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1368,7 +1368,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>SUS</t>
+          <t>Não SUS</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1378,11 +1378,11 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>01/01/2012</t>
+          <t>01/01/2024</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>78.27902663144874</v>
+        <v>2.375456636863682</v>
       </c>
     </row>
     <row r="39">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>SUS</t>
+          <t>Não SUS</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1403,11 +1403,11 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>01/01/2012</t>
+          <t>01/01/2024</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>22.63218361558187</v>
+        <v>40.84627776510756</v>
       </c>
     </row>
     <row r="40">
@@ -1418,7 +1418,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>SUS</t>
+          <t>Não SUS</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1428,11 +1428,11 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>01/01/2012</t>
+          <t>01/01/2024</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>63.50555525989787</v>
+        <v>21.60788122764592</v>
       </c>
     </row>
     <row r="41">
@@ -1453,11 +1453,11 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>01/01/2013</t>
+          <t>01/01/2012</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>78.01886628493999</v>
+        <v>78.27902663144874</v>
       </c>
     </row>
     <row r="42">
@@ -1478,11 +1478,11 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>01/01/2013</t>
+          <t>01/01/2012</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>20.60206859268367</v>
+        <v>22.63218361558187</v>
       </c>
     </row>
     <row r="43">
@@ -1503,11 +1503,11 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>01/01/2013</t>
+          <t>01/01/2012</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>62.08219999873203</v>
+        <v>63.50555525989787</v>
       </c>
     </row>
     <row r="44">
@@ -1528,11 +1528,11 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>01/01/2014</t>
+          <t>01/01/2013</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>78.93859860209182</v>
+        <v>78.01886628493999</v>
       </c>
     </row>
     <row r="45">
@@ -1553,11 +1553,11 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>01/01/2014</t>
+          <t>01/01/2013</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>18.50012637225237</v>
+        <v>20.60206859268367</v>
       </c>
     </row>
     <row r="46">
@@ -1578,11 +1578,11 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>01/01/2014</t>
+          <t>01/01/2013</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>60.84349402216835</v>
+        <v>62.08219999873203</v>
       </c>
     </row>
     <row r="47">
@@ -1603,11 +1603,11 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>01/01/2015</t>
+          <t>01/01/2014</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>78.39806587600937</v>
+        <v>78.93859860209182</v>
       </c>
     </row>
     <row r="48">
@@ -1628,11 +1628,11 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>01/01/2015</t>
+          <t>01/01/2014</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>15.99404878272358</v>
+        <v>18.50012637225237</v>
       </c>
     </row>
     <row r="49">
@@ -1653,11 +1653,11 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>01/01/2015</t>
+          <t>01/01/2014</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>58.90237016675845</v>
+        <v>60.84349402216835</v>
       </c>
     </row>
     <row r="50">
@@ -1678,11 +1678,11 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>01/01/2016</t>
+          <t>01/01/2015</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>79.26530772321729</v>
+        <v>78.39806587600937</v>
       </c>
     </row>
     <row r="51">
@@ -1703,11 +1703,11 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>01/01/2016</t>
+          <t>01/01/2015</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>14.35098937378988</v>
+        <v>15.99404878272358</v>
       </c>
     </row>
     <row r="52">
@@ -1728,11 +1728,11 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>01/01/2016</t>
+          <t>01/01/2015</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>56.41788143024625</v>
+        <v>58.90237016675845</v>
       </c>
     </row>
     <row r="53">
@@ -1753,11 +1753,11 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>01/01/2017</t>
+          <t>01/01/2016</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>78.89567676787448</v>
+        <v>79.26530772321729</v>
       </c>
     </row>
     <row r="54">
@@ -1778,11 +1778,11 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>01/01/2017</t>
+          <t>01/01/2016</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>12.99341585210563</v>
+        <v>14.35098937378988</v>
       </c>
     </row>
     <row r="55">
@@ -1803,11 +1803,11 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>01/01/2017</t>
+          <t>01/01/2016</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>54.7144129543916</v>
+        <v>56.41788143024625</v>
       </c>
     </row>
     <row r="56">
@@ -1828,11 +1828,11 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>01/01/2018</t>
+          <t>01/01/2017</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>77.37407485746654</v>
+        <v>78.89567676787448</v>
       </c>
     </row>
     <row r="57">
@@ -1853,11 +1853,11 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>01/01/2018</t>
+          <t>01/01/2017</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>11.59980411990893</v>
+        <v>12.99341585210563</v>
       </c>
     </row>
     <row r="58">
@@ -1878,11 +1878,11 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>01/01/2018</t>
+          <t>01/01/2017</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>55.04882853249648</v>
+        <v>54.7144129543916</v>
       </c>
     </row>
     <row r="59">
@@ -1903,11 +1903,11 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>01/01/2019</t>
+          <t>01/01/2018</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>76.42788356014863</v>
+        <v>77.37407485746654</v>
       </c>
     </row>
     <row r="60">
@@ -1928,11 +1928,11 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>01/01/2019</t>
+          <t>01/01/2018</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>10.28517520760753</v>
+        <v>11.59980411990893</v>
       </c>
     </row>
     <row r="61">
@@ -1953,11 +1953,11 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>01/01/2019</t>
+          <t>01/01/2018</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>53.64955623351973</v>
+        <v>55.04882853249648</v>
       </c>
     </row>
     <row r="62">
@@ -1978,11 +1978,11 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
+          <t>01/01/2019</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>82.58148734910984</v>
+        <v>76.42788356014863</v>
       </c>
     </row>
     <row r="63">
@@ -2003,11 +2003,11 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
+          <t>01/01/2019</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>10.84835065496138</v>
+        <v>10.28517520760753</v>
       </c>
     </row>
     <row r="64">
@@ -2028,11 +2028,11 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
+          <t>01/01/2019</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>54.39995445317238</v>
+        <v>53.64955623351973</v>
       </c>
     </row>
     <row r="65">
@@ -2053,11 +2053,11 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
+          <t>01/01/2020</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>80.98111380278309</v>
+        <v>82.58148734910984</v>
       </c>
     </row>
     <row r="66">
@@ -2078,11 +2078,11 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
+          <t>01/01/2020</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>10.55890178870768</v>
+        <v>10.84835065496138</v>
       </c>
     </row>
     <row r="67">
@@ -2103,11 +2103,11 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
+          <t>01/01/2020</t>
         </is>
       </c>
       <c r="E67" t="n">
-        <v>53.9908469547612</v>
+        <v>54.39995445317238</v>
       </c>
     </row>
     <row r="68">
@@ -2128,11 +2128,11 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
+          <t>01/01/2021</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>80.70296432680685</v>
+        <v>80.98111380278309</v>
       </c>
     </row>
     <row r="69">
@@ -2153,11 +2153,11 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
+          <t>01/01/2021</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>10.41528281111997</v>
+        <v>10.55890178870768</v>
       </c>
     </row>
     <row r="70">
@@ -2178,11 +2178,11 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
+          <t>01/01/2021</t>
         </is>
       </c>
       <c r="E70" t="n">
-        <v>52.9403588554854</v>
+        <v>53.9908469547612</v>
       </c>
     </row>
     <row r="71">
@@ -2203,11 +2203,11 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>01/01/2023</t>
+          <t>01/01/2022</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>80.05713998552525</v>
+        <v>80.70296432680685</v>
       </c>
     </row>
     <row r="72">
@@ -2228,11 +2228,11 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>01/01/2023</t>
+          <t>01/01/2022</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>10.4020510155549</v>
+        <v>10.41528281111997</v>
       </c>
     </row>
     <row r="73">
@@ -2253,22 +2253,22 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>01/01/2023</t>
+          <t>01/01/2022</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>52.68852909501246</v>
+        <v>52.9403588554854</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Nordeste</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Não SUS</t>
+          <t>SUS</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2278,20 +2278,22 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>01/01/2012</t>
-        </is>
-      </c>
-      <c r="E74" t="inlineStr"/>
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="E74" t="n">
+        <v>80.05713998552525</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Nordeste</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Não SUS</t>
+          <t>SUS</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2301,20 +2303,22 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>01/01/2012</t>
-        </is>
-      </c>
-      <c r="E75" t="inlineStr"/>
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="E75" t="n">
+        <v>10.4020510155549</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Nordeste</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Não SUS</t>
+          <t>SUS</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2324,20 +2328,22 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>01/01/2012</t>
-        </is>
-      </c>
-      <c r="E76" t="inlineStr"/>
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="E76" t="n">
+        <v>52.68852909501246</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Nordeste</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Não SUS</t>
+          <t>SUS</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2347,20 +2353,22 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>01/01/2013</t>
-        </is>
-      </c>
-      <c r="E77" t="inlineStr"/>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="E77" t="n">
+        <v>80.38607734896577</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Nordeste</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Não SUS</t>
+          <t>SUS</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2370,20 +2378,22 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>01/01/2013</t>
-        </is>
-      </c>
-      <c r="E78" t="inlineStr"/>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="E78" t="n">
+        <v>10.17573776120043</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Nordeste</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Não SUS</t>
+          <t>SUS</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2393,10 +2403,12 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>01/01/2013</t>
-        </is>
-      </c>
-      <c r="E79" t="inlineStr"/>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="E79" t="n">
+        <v>53.63589064983426</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2416,10 +2428,12 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>01/01/2014</t>
-        </is>
-      </c>
-      <c r="E80" t="inlineStr"/>
+          <t>01/01/2012</t>
+        </is>
+      </c>
+      <c r="E80" t="n">
+        <v>1.363004209970142</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -2439,10 +2453,12 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>01/01/2014</t>
-        </is>
-      </c>
-      <c r="E81" t="inlineStr"/>
+          <t>01/01/2012</t>
+        </is>
+      </c>
+      <c r="E81" t="n">
+        <v>26.84826741938513</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -2462,10 +2478,12 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>01/01/2014</t>
-        </is>
-      </c>
-      <c r="E82" t="inlineStr"/>
+          <t>01/01/2012</t>
+        </is>
+      </c>
+      <c r="E82" t="n">
+        <v>7.636832411744475</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -2485,10 +2503,12 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>01/01/2015</t>
-        </is>
-      </c>
-      <c r="E83" t="inlineStr"/>
+          <t>01/01/2013</t>
+        </is>
+      </c>
+      <c r="E83" t="n">
+        <v>1.393404366635746</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -2508,10 +2528,12 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>01/01/2015</t>
-        </is>
-      </c>
-      <c r="E84" t="inlineStr"/>
+          <t>01/01/2013</t>
+        </is>
+      </c>
+      <c r="E84" t="n">
+        <v>26.48917872021843</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -2531,10 +2553,12 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>01/01/2015</t>
-        </is>
-      </c>
-      <c r="E85" t="inlineStr"/>
+          <t>01/01/2013</t>
+        </is>
+      </c>
+      <c r="E85" t="n">
+        <v>7.813211481057654</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -2554,10 +2578,12 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>01/01/2016</t>
-        </is>
-      </c>
-      <c r="E86" t="inlineStr"/>
+          <t>01/01/2014</t>
+        </is>
+      </c>
+      <c r="E86" t="n">
+        <v>1.540517779737308</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -2577,10 +2603,12 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>01/01/2016</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr"/>
+          <t>01/01/2014</t>
+        </is>
+      </c>
+      <c r="E87" t="n">
+        <v>27.57436736970733</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -2600,10 +2628,12 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>01/01/2016</t>
-        </is>
-      </c>
-      <c r="E88" t="inlineStr"/>
+          <t>01/01/2014</t>
+        </is>
+      </c>
+      <c r="E88" t="n">
+        <v>7.154849243668832</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -2623,10 +2653,12 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>01/01/2017</t>
-        </is>
-      </c>
-      <c r="E89" t="inlineStr"/>
+          <t>01/01/2015</t>
+        </is>
+      </c>
+      <c r="E89" t="n">
+        <v>1.467000705772427</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -2646,10 +2678,12 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>01/01/2017</t>
-        </is>
-      </c>
-      <c r="E90" t="inlineStr"/>
+          <t>01/01/2015</t>
+        </is>
+      </c>
+      <c r="E90" t="n">
+        <v>27.20310099946991</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -2669,10 +2703,12 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>01/01/2017</t>
-        </is>
-      </c>
-      <c r="E91" t="inlineStr"/>
+          <t>01/01/2015</t>
+        </is>
+      </c>
+      <c r="E91" t="n">
+        <v>7.870575215096516</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -2692,10 +2728,12 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>01/01/2018</t>
-        </is>
-      </c>
-      <c r="E92" t="inlineStr"/>
+          <t>01/01/2016</t>
+        </is>
+      </c>
+      <c r="E92" t="n">
+        <v>1.55330093370843</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -2715,10 +2753,12 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>01/01/2018</t>
-        </is>
-      </c>
-      <c r="E93" t="inlineStr"/>
+          <t>01/01/2016</t>
+        </is>
+      </c>
+      <c r="E93" t="n">
+        <v>27.75812895639731</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -2738,10 +2778,12 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>01/01/2018</t>
-        </is>
-      </c>
-      <c r="E94" t="inlineStr"/>
+          <t>01/01/2016</t>
+        </is>
+      </c>
+      <c r="E94" t="n">
+        <v>7.949979434794405</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -2761,10 +2803,12 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>01/01/2019</t>
-        </is>
-      </c>
-      <c r="E95" t="inlineStr"/>
+          <t>01/01/2017</t>
+        </is>
+      </c>
+      <c r="E95" t="n">
+        <v>1.475847420338301</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -2784,10 +2828,12 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>01/01/2019</t>
-        </is>
-      </c>
-      <c r="E96" t="inlineStr"/>
+          <t>01/01/2017</t>
+        </is>
+      </c>
+      <c r="E96" t="n">
+        <v>29.88369560485729</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -2807,10 +2853,12 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>01/01/2019</t>
-        </is>
-      </c>
-      <c r="E97" t="inlineStr"/>
+          <t>01/01/2017</t>
+        </is>
+      </c>
+      <c r="E97" t="n">
+        <v>8.736378907188669</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -2830,10 +2878,12 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
-        </is>
-      </c>
-      <c r="E98" t="inlineStr"/>
+          <t>01/01/2018</t>
+        </is>
+      </c>
+      <c r="E98" t="n">
+        <v>1.421756360641979</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -2853,10 +2903,12 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
-        </is>
-      </c>
-      <c r="E99" t="inlineStr"/>
+          <t>01/01/2018</t>
+        </is>
+      </c>
+      <c r="E99" t="n">
+        <v>28.52673976643732</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -2876,10 +2928,12 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
-        </is>
-      </c>
-      <c r="E100" t="inlineStr"/>
+          <t>01/01/2018</t>
+        </is>
+      </c>
+      <c r="E100" t="n">
+        <v>8.201085326875353</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -2899,10 +2953,12 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
-        </is>
-      </c>
-      <c r="E101" t="inlineStr"/>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="E101" t="n">
+        <v>1.331659320754923</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -2922,10 +2978,12 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
-        </is>
-      </c>
-      <c r="E102" t="inlineStr"/>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="E102" t="n">
+        <v>31.00488379047153</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -2945,10 +3003,12 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
-        </is>
-      </c>
-      <c r="E103" t="inlineStr"/>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="E103" t="n">
+        <v>7.94615134160997</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -2968,10 +3028,12 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
-        </is>
-      </c>
-      <c r="E104" t="inlineStr"/>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+      <c r="E104" t="n">
+        <v>1.732484731868271</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -2991,10 +3053,12 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
-        </is>
-      </c>
-      <c r="E105" t="inlineStr"/>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+      <c r="E105" t="n">
+        <v>31.58908780722388</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -3014,10 +3078,12 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
-        </is>
-      </c>
-      <c r="E106" t="inlineStr"/>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+      <c r="E106" t="n">
+        <v>7.707291231711763</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -3037,10 +3103,12 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>01/01/2023</t>
-        </is>
-      </c>
-      <c r="E107" t="inlineStr"/>
+          <t>01/01/2021</t>
+        </is>
+      </c>
+      <c r="E107" t="n">
+        <v>1.690716985733574</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -3060,10 +3128,12 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>01/01/2023</t>
-        </is>
-      </c>
-      <c r="E108" t="inlineStr"/>
+          <t>01/01/2021</t>
+        </is>
+      </c>
+      <c r="E108" t="n">
+        <v>32.65598182085607</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -3083,10 +3153,12 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>01/01/2023</t>
-        </is>
-      </c>
-      <c r="E109" t="inlineStr"/>
+          <t>01/01/2021</t>
+        </is>
+      </c>
+      <c r="E109" t="n">
+        <v>7.870937844353532</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -3096,7 +3168,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>SUS</t>
+          <t>Não SUS</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -3106,10 +3178,12 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>01/01/2012</t>
-        </is>
-      </c>
-      <c r="E110" t="inlineStr"/>
+          <t>01/01/2022</t>
+        </is>
+      </c>
+      <c r="E110" t="n">
+        <v>1.685897430034868</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -3119,7 +3193,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>SUS</t>
+          <t>Não SUS</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -3129,10 +3203,12 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>01/01/2012</t>
-        </is>
-      </c>
-      <c r="E111" t="inlineStr"/>
+          <t>01/01/2022</t>
+        </is>
+      </c>
+      <c r="E111" t="n">
+        <v>34.1165589449533</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -3142,7 +3218,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>SUS</t>
+          <t>Não SUS</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -3152,10 +3228,12 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>01/01/2012</t>
-        </is>
-      </c>
-      <c r="E112" t="inlineStr"/>
+          <t>01/01/2022</t>
+        </is>
+      </c>
+      <c r="E112" t="n">
+        <v>8.03950473544775</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -3165,7 +3243,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>SUS</t>
+          <t>Não SUS</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -3175,10 +3253,12 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>01/01/2013</t>
-        </is>
-      </c>
-      <c r="E113" t="inlineStr"/>
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="E113" t="n">
+        <v>1.509695102217608</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -3188,7 +3268,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>SUS</t>
+          <t>Não SUS</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -3198,10 +3278,12 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>01/01/2013</t>
-        </is>
-      </c>
-      <c r="E114" t="inlineStr"/>
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="E114" t="n">
+        <v>34.90676138506333</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -3211,7 +3293,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>SUS</t>
+          <t>Não SUS</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -3221,10 +3303,12 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>01/01/2013</t>
-        </is>
-      </c>
-      <c r="E115" t="inlineStr"/>
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="E115" t="n">
+        <v>8.692340059525955</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -3234,7 +3318,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>SUS</t>
+          <t>Não SUS</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -3244,10 +3328,12 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>01/01/2014</t>
-        </is>
-      </c>
-      <c r="E116" t="inlineStr"/>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="E116" t="n">
+        <v>1.491002161029807</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -3257,7 +3343,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>SUS</t>
+          <t>Não SUS</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -3267,10 +3353,12 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>01/01/2014</t>
-        </is>
-      </c>
-      <c r="E117" t="inlineStr"/>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="E117" t="n">
+        <v>35.08984673010744</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -3280,7 +3368,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>SUS</t>
+          <t>Não SUS</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -3290,10 +3378,12 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>01/01/2014</t>
-        </is>
-      </c>
-      <c r="E118" t="inlineStr"/>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="E118" t="n">
+        <v>8.152635669484079</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -3313,10 +3403,12 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>01/01/2015</t>
-        </is>
-      </c>
-      <c r="E119" t="inlineStr"/>
+          <t>01/01/2012</t>
+        </is>
+      </c>
+      <c r="E119" t="n">
+        <v>107.1361397395649</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -3336,10 +3428,12 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>01/01/2015</t>
-        </is>
-      </c>
-      <c r="E120" t="inlineStr"/>
+          <t>01/01/2012</t>
+        </is>
+      </c>
+      <c r="E120" t="n">
+        <v>28.0254074189048</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -3359,10 +3453,12 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>01/01/2015</t>
-        </is>
-      </c>
-      <c r="E121" t="inlineStr"/>
+          <t>01/01/2012</t>
+        </is>
+      </c>
+      <c r="E121" t="n">
+        <v>44.5600333564303</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -3382,10 +3478,12 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>01/01/2016</t>
-        </is>
-      </c>
-      <c r="E122" t="inlineStr"/>
+          <t>01/01/2013</t>
+        </is>
+      </c>
+      <c r="E122" t="n">
+        <v>108.310462959235</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -3405,10 +3503,12 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>01/01/2016</t>
-        </is>
-      </c>
-      <c r="E123" t="inlineStr"/>
+          <t>01/01/2013</t>
+        </is>
+      </c>
+      <c r="E123" t="n">
+        <v>25.49621956167956</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -3428,10 +3528,12 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>01/01/2016</t>
-        </is>
-      </c>
-      <c r="E124" t="inlineStr"/>
+          <t>01/01/2013</t>
+        </is>
+      </c>
+      <c r="E124" t="n">
+        <v>43.14117628768592</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -3451,10 +3553,12 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>01/01/2017</t>
-        </is>
-      </c>
-      <c r="E125" t="inlineStr"/>
+          <t>01/01/2014</t>
+        </is>
+      </c>
+      <c r="E125" t="n">
+        <v>109.9551321944433</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -3474,10 +3578,12 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>01/01/2017</t>
-        </is>
-      </c>
-      <c r="E126" t="inlineStr"/>
+          <t>01/01/2014</t>
+        </is>
+      </c>
+      <c r="E126" t="n">
+        <v>22.97803888302911</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -3497,10 +3603,12 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>01/01/2017</t>
-        </is>
-      </c>
-      <c r="E127" t="inlineStr"/>
+          <t>01/01/2014</t>
+        </is>
+      </c>
+      <c r="E127" t="n">
+        <v>41.00660134390807</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -3520,10 +3628,12 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>01/01/2018</t>
-        </is>
-      </c>
-      <c r="E128" t="inlineStr"/>
+          <t>01/01/2015</t>
+        </is>
+      </c>
+      <c r="E128" t="n">
+        <v>109.3408108455022</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -3543,10 +3653,12 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>01/01/2018</t>
-        </is>
-      </c>
-      <c r="E129" t="inlineStr"/>
+          <t>01/01/2015</t>
+        </is>
+      </c>
+      <c r="E129" t="n">
+        <v>20.21738335293454</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -3566,10 +3678,12 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>01/01/2018</t>
-        </is>
-      </c>
-      <c r="E130" t="inlineStr"/>
+          <t>01/01/2015</t>
+        </is>
+      </c>
+      <c r="E130" t="n">
+        <v>39.19166720671638</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -3589,10 +3703,12 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>01/01/2019</t>
-        </is>
-      </c>
-      <c r="E131" t="inlineStr"/>
+          <t>01/01/2016</t>
+        </is>
+      </c>
+      <c r="E131" t="n">
+        <v>111.0699233022038</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -3612,10 +3728,12 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>01/01/2019</t>
-        </is>
-      </c>
-      <c r="E132" t="inlineStr"/>
+          <t>01/01/2016</t>
+        </is>
+      </c>
+      <c r="E132" t="n">
+        <v>18.38488410184025</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -3635,10 +3753,12 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>01/01/2019</t>
-        </is>
-      </c>
-      <c r="E133" t="inlineStr"/>
+          <t>01/01/2016</t>
+        </is>
+      </c>
+      <c r="E133" t="n">
+        <v>37.65864110037833</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -3658,10 +3778,12 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
-        </is>
-      </c>
-      <c r="E134" t="inlineStr"/>
+          <t>01/01/2017</t>
+        </is>
+      </c>
+      <c r="E134" t="n">
+        <v>111.8277760827285</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -3681,10 +3803,12 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
-        </is>
-      </c>
-      <c r="E135" t="inlineStr"/>
+          <t>01/01/2017</t>
+        </is>
+      </c>
+      <c r="E135" t="n">
+        <v>17.65524555062565</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -3704,10 +3828,12 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
-        </is>
-      </c>
-      <c r="E136" t="inlineStr"/>
+          <t>01/01/2017</t>
+        </is>
+      </c>
+      <c r="E136" t="n">
+        <v>36.35580920209116</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -3727,10 +3853,12 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
-        </is>
-      </c>
-      <c r="E137" t="inlineStr"/>
+          <t>01/01/2018</t>
+        </is>
+      </c>
+      <c r="E137" t="n">
+        <v>111.4889541687059</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -3750,10 +3878,12 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
-        </is>
-      </c>
-      <c r="E138" t="inlineStr"/>
+          <t>01/01/2018</t>
+        </is>
+      </c>
+      <c r="E138" t="n">
+        <v>15.58646657075537</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -3773,10 +3903,12 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
-        </is>
-      </c>
-      <c r="E139" t="inlineStr"/>
+          <t>01/01/2018</t>
+        </is>
+      </c>
+      <c r="E139" t="n">
+        <v>35.80289065795079</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -3796,10 +3928,12 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
-        </is>
-      </c>
-      <c r="E140" t="inlineStr"/>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="E140" t="n">
+        <v>110.5995631386467</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -3819,10 +3953,12 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
-        </is>
-      </c>
-      <c r="E141" t="inlineStr"/>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="E141" t="n">
+        <v>14.51508659622866</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -3842,10 +3978,12 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
-        </is>
-      </c>
-      <c r="E142" t="inlineStr"/>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="E142" t="n">
+        <v>35.23991086713555</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -3865,10 +4003,12 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>01/01/2023</t>
-        </is>
-      </c>
-      <c r="E143" t="inlineStr"/>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+      <c r="E143" t="n">
+        <v>120.1410186797584</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -3888,10 +4028,12 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>01/01/2023</t>
-        </is>
-      </c>
-      <c r="E144" t="inlineStr"/>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+      <c r="E144" t="n">
+        <v>15.45989896546435</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -3911,20 +4053,22 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>01/01/2023</t>
-        </is>
-      </c>
-      <c r="E145" t="inlineStr"/>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+      <c r="E145" t="n">
+        <v>35.48804992512058</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Não SUS</t>
+          <t>SUS</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -3934,22 +4078,22 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>01/01/2012</t>
+          <t>01/01/2021</t>
         </is>
       </c>
       <c r="E146" t="n">
-        <v>2.880600502990017</v>
+        <v>120.6096805217716</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Não SUS</t>
+          <t>SUS</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -3959,22 +4103,22 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>01/01/2012</t>
+          <t>01/01/2021</t>
         </is>
       </c>
       <c r="E147" t="n">
-        <v>28.062624254935</v>
+        <v>15.02397124553404</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Não SUS</t>
+          <t>SUS</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -3984,22 +4128,22 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>01/01/2012</t>
+          <t>01/01/2021</t>
         </is>
       </c>
       <c r="E148" t="n">
-        <v>4.274439456049703</v>
+        <v>34.42820003564552</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Não SUS</t>
+          <t>SUS</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -4009,22 +4153,22 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>01/01/2013</t>
+          <t>01/01/2022</t>
         </is>
       </c>
       <c r="E149" t="n">
-        <v>2.852368754232547</v>
+        <v>119.3346189063371</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Não SUS</t>
+          <t>SUS</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -4034,22 +4178,22 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>01/01/2013</t>
+          <t>01/01/2022</t>
         </is>
       </c>
       <c r="E150" t="n">
-        <v>27.78759237994288</v>
+        <v>15.06263937233814</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Não SUS</t>
+          <t>SUS</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -4059,22 +4203,22 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>01/01/2013</t>
+          <t>01/01/2022</t>
         </is>
       </c>
       <c r="E151" t="n">
-        <v>4.186541236050997</v>
+        <v>33.5212318074282</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Não SUS</t>
+          <t>SUS</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -4084,22 +4228,22 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>01/01/2014</t>
+          <t>01/01/2023</t>
         </is>
       </c>
       <c r="E152" t="n">
-        <v>2.870139839591073</v>
+        <v>118.6716531145912</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Não SUS</t>
+          <t>SUS</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -4109,22 +4253,22 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>01/01/2014</t>
+          <t>01/01/2023</t>
         </is>
       </c>
       <c r="E153" t="n">
-        <v>27.51689623988902</v>
+        <v>14.62463457950277</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Não SUS</t>
+          <t>SUS</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -4134,22 +4278,22 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>01/01/2014</t>
+          <t>01/01/2023</t>
         </is>
       </c>
       <c r="E154" t="n">
-        <v>3.234602041443908</v>
+        <v>33.02093064304407</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Não SUS</t>
+          <t>SUS</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -4159,22 +4303,22 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>01/01/2015</t>
+          <t>01/01/2024</t>
         </is>
       </c>
       <c r="E155" t="n">
-        <v>2.79700467866702</v>
+        <v>119.2989813958837</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Não SUS</t>
+          <t>SUS</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -4184,22 +4328,22 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>01/01/2015</t>
+          <t>01/01/2024</t>
         </is>
       </c>
       <c r="E156" t="n">
-        <v>27.11290019159482</v>
+        <v>14.73903512394144</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Não SUS</t>
+          <t>SUS</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -4209,11 +4353,11 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>01/01/2015</t>
+          <t>01/01/2024</t>
         </is>
       </c>
       <c r="E157" t="n">
-        <v>4.015055103247819</v>
+        <v>32.72168389406813</v>
       </c>
     </row>
     <row r="158">
@@ -4234,11 +4378,11 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>01/01/2016</t>
+          <t>01/01/2012</t>
         </is>
       </c>
       <c r="E158" t="n">
-        <v>3.307806602381978</v>
+        <v>2.880600502990017</v>
       </c>
     </row>
     <row r="159">
@@ -4259,11 +4403,11 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>01/01/2016</t>
+          <t>01/01/2012</t>
         </is>
       </c>
       <c r="E159" t="n">
-        <v>27.71405531725441</v>
+        <v>28.062624254935</v>
       </c>
     </row>
     <row r="160">
@@ -4284,11 +4428,11 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>01/01/2016</t>
+          <t>01/01/2012</t>
         </is>
       </c>
       <c r="E160" t="n">
-        <v>4.648809279023321</v>
+        <v>4.274439456049703</v>
       </c>
     </row>
     <row r="161">
@@ -4309,11 +4453,11 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>01/01/2017</t>
+          <t>01/01/2013</t>
         </is>
       </c>
       <c r="E161" t="n">
-        <v>3.455507680530341</v>
+        <v>2.852368754232547</v>
       </c>
     </row>
     <row r="162">
@@ -4334,11 +4478,11 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>01/01/2017</t>
+          <t>01/01/2013</t>
         </is>
       </c>
       <c r="E162" t="n">
-        <v>27.64406144424273</v>
+        <v>27.78759237994288</v>
       </c>
     </row>
     <row r="163">
@@ -4359,11 +4503,11 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>01/01/2017</t>
+          <t>01/01/2013</t>
         </is>
       </c>
       <c r="E163" t="n">
-        <v>3.987124246765778</v>
+        <v>4.186541236050997</v>
       </c>
     </row>
     <row r="164">
@@ -4384,11 +4528,11 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>01/01/2018</t>
+          <t>01/01/2014</t>
         </is>
       </c>
       <c r="E164" t="n">
-        <v>3.423593298184442</v>
+        <v>2.870139839591073</v>
       </c>
     </row>
     <row r="165">
@@ -4409,11 +4553,11 @@
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>01/01/2018</t>
+          <t>01/01/2014</t>
         </is>
       </c>
       <c r="E165" t="n">
-        <v>26.46700972827203</v>
+        <v>27.51689623988902</v>
       </c>
     </row>
     <row r="166">
@@ -4434,11 +4578,11 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>01/01/2018</t>
+          <t>01/01/2014</t>
         </is>
       </c>
       <c r="E166" t="n">
-        <v>5.530419943221021</v>
+        <v>3.234602041443908</v>
       </c>
     </row>
     <row r="167">
@@ -4459,11 +4603,11 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>01/01/2019</t>
+          <t>01/01/2015</t>
         </is>
       </c>
       <c r="E167" t="n">
-        <v>3.392924100287876</v>
+        <v>2.79700467866702</v>
       </c>
     </row>
     <row r="168">
@@ -4484,11 +4628,11 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>01/01/2019</t>
+          <t>01/01/2015</t>
         </is>
       </c>
       <c r="E168" t="n">
-        <v>28.75285679859342</v>
+        <v>27.11290019159482</v>
       </c>
     </row>
     <row r="169">
@@ -4509,11 +4653,11 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>01/01/2019</t>
+          <t>01/01/2015</t>
         </is>
       </c>
       <c r="E169" t="n">
-        <v>4.958889069651512</v>
+        <v>4.015055103247819</v>
       </c>
     </row>
     <row r="170">
@@ -4534,11 +4678,11 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
+          <t>01/01/2016</t>
         </is>
       </c>
       <c r="E170" t="n">
-        <v>2.846015061456677</v>
+        <v>3.307806602381978</v>
       </c>
     </row>
     <row r="171">
@@ -4559,11 +4703,11 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
+          <t>01/01/2016</t>
         </is>
       </c>
       <c r="E171" t="n">
-        <v>28.46015061456677</v>
+        <v>27.71405531725441</v>
       </c>
     </row>
     <row r="172">
@@ -4584,11 +4728,11 @@
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
+          <t>01/01/2016</t>
         </is>
       </c>
       <c r="E172" t="n">
-        <v>5.433301480962746</v>
+        <v>4.648809279023321</v>
       </c>
     </row>
     <row r="173">
@@ -4609,11 +4753,11 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
+          <t>01/01/2017</t>
         </is>
       </c>
       <c r="E173" t="n">
-        <v>2.822095123419627</v>
+        <v>3.455507680530341</v>
       </c>
     </row>
     <row r="174">
@@ -4634,11 +4778,11 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
+          <t>01/01/2017</t>
         </is>
       </c>
       <c r="E174" t="n">
-        <v>29.58923977888457</v>
+        <v>27.64406144424273</v>
       </c>
     </row>
     <row r="175">
@@ -4659,11 +4803,11 @@
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
+          <t>01/01/2017</t>
         </is>
       </c>
       <c r="E175" t="n">
-        <v>5.387636144710196</v>
+        <v>3.987124246765778</v>
       </c>
     </row>
     <row r="176">
@@ -4684,11 +4828,11 @@
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
+          <t>01/01/2018</t>
         </is>
       </c>
       <c r="E176" t="n">
-        <v>0.8058222780171683</v>
+        <v>3.423593298184442</v>
       </c>
     </row>
     <row r="177">
@@ -4709,11 +4853,11 @@
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
+          <t>01/01/2018</t>
         </is>
       </c>
       <c r="E177" t="n">
-        <v>30.49401146812337</v>
+        <v>26.46700972827203</v>
       </c>
     </row>
     <row r="178">
@@ -4734,11 +4878,11 @@
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
+          <t>01/01/2018</t>
         </is>
       </c>
       <c r="E178" t="n">
-        <v>6.31934312760832</v>
+        <v>5.530419943221021</v>
       </c>
     </row>
     <row r="179">
@@ -4759,11 +4903,11 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>01/01/2023</t>
+          <t>01/01/2019</t>
         </is>
       </c>
       <c r="E179" t="n">
-        <v>1.556946146915963</v>
+        <v>3.392924100287876</v>
       </c>
     </row>
     <row r="180">
@@ -4784,11 +4928,11 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>01/01/2023</t>
+          <t>01/01/2019</t>
         </is>
       </c>
       <c r="E180" t="n">
-        <v>26.63640299994067</v>
+        <v>28.75285679859342</v>
       </c>
     </row>
     <row r="181">
@@ -4809,11 +4953,11 @@
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>01/01/2023</t>
+          <t>01/01/2019</t>
         </is>
       </c>
       <c r="E181" t="n">
-        <v>6.985217848325673</v>
+        <v>4.958889069651512</v>
       </c>
     </row>
     <row r="182">
@@ -4824,7 +4968,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>SUS</t>
+          <t>Não SUS</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
@@ -4834,11 +4978,11 @@
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>01/01/2012</t>
+          <t>01/01/2020</t>
         </is>
       </c>
       <c r="E182" t="n">
-        <v>17.8875998975993</v>
+        <v>2.846015061456677</v>
       </c>
     </row>
     <row r="183">
@@ -4849,7 +4993,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>SUS</t>
+          <t>Não SUS</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -4859,11 +5003,11 @@
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>01/01/2012</t>
+          <t>01/01/2020</t>
         </is>
       </c>
       <c r="E183" t="n">
-        <v>15.75038016957445</v>
+        <v>28.46015061456677</v>
       </c>
     </row>
     <row r="184">
@@ -4874,7 +5018,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>SUS</t>
+          <t>Não SUS</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
@@ -4884,11 +5028,11 @@
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>01/01/2012</t>
+          <t>01/01/2020</t>
         </is>
       </c>
       <c r="E184" t="n">
-        <v>99.42717865159091</v>
+        <v>5.433301480962746</v>
       </c>
     </row>
     <row r="185">
@@ -4899,7 +5043,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>SUS</t>
+          <t>Não SUS</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
@@ -4909,11 +5053,11 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>01/01/2013</t>
+          <t>01/01/2021</t>
         </is>
       </c>
       <c r="E185" t="n">
-        <v>14.58388540470512</v>
+        <v>2.822095123419627</v>
       </c>
     </row>
     <row r="186">
@@ -4924,7 +5068,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>SUS</t>
+          <t>Não SUS</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
@@ -4934,11 +5078,11 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>01/01/2013</t>
+          <t>01/01/2021</t>
         </is>
       </c>
       <c r="E186" t="n">
-        <v>12.83565939404646</v>
+        <v>29.58923977888457</v>
       </c>
     </row>
     <row r="187">
@@ -4949,7 +5093,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>SUS</t>
+          <t>Não SUS</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
@@ -4959,11 +5103,11 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>01/01/2013</t>
+          <t>01/01/2021</t>
         </is>
       </c>
       <c r="E187" t="n">
-        <v>96.9805376439066</v>
+        <v>5.387636144710196</v>
       </c>
     </row>
     <row r="188">
@@ -4974,7 +5118,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>SUS</t>
+          <t>Não SUS</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
@@ -4984,11 +5128,11 @@
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>01/01/2014</t>
+          <t>01/01/2022</t>
         </is>
       </c>
       <c r="E188" t="n">
-        <v>46.33225741054162</v>
+        <v>0.8058222780171683</v>
       </c>
     </row>
     <row r="189">
@@ -4999,7 +5143,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>SUS</t>
+          <t>Não SUS</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
@@ -5009,11 +5153,11 @@
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>01/01/2014</t>
+          <t>01/01/2022</t>
         </is>
       </c>
       <c r="E189" t="n">
-        <v>18.04087899171532</v>
+        <v>30.49401146812337</v>
       </c>
     </row>
     <row r="190">
@@ -5024,7 +5168,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>SUS</t>
+          <t>Não SUS</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
@@ -5034,11 +5178,11 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>01/01/2014</t>
+          <t>01/01/2022</t>
         </is>
       </c>
       <c r="E190" t="n">
-        <v>55.7171591082521</v>
+        <v>6.31934312760832</v>
       </c>
     </row>
     <row r="191">
@@ -5049,7 +5193,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>SUS</t>
+          <t>Não SUS</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
@@ -5059,11 +5203,11 @@
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>01/01/2015</t>
+          <t>01/01/2023</t>
         </is>
       </c>
       <c r="E191" t="n">
-        <v>54.76715612744778</v>
+        <v>1.556946146915963</v>
       </c>
     </row>
     <row r="192">
@@ -5074,7 +5218,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>SUS</t>
+          <t>Não SUS</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
@@ -5084,11 +5228,11 @@
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>01/01/2015</t>
+          <t>01/01/2023</t>
         </is>
       </c>
       <c r="E192" t="n">
-        <v>10.64666297040995</v>
+        <v>26.63640299994067</v>
       </c>
     </row>
     <row r="193">
@@ -5099,7 +5243,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>SUS</t>
+          <t>Não SUS</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
@@ -5109,11 +5253,11 @@
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>01/01/2015</t>
+          <t>01/01/2023</t>
         </is>
       </c>
       <c r="E193" t="n">
-        <v>43.39868549802699</v>
+        <v>6.985217848325673</v>
       </c>
     </row>
     <row r="194">
@@ -5124,7 +5268,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>SUS</t>
+          <t>Não SUS</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
@@ -5134,11 +5278,11 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>01/01/2016</t>
+          <t>01/01/2024</t>
         </is>
       </c>
       <c r="E194" t="n">
-        <v>55.02580983151642</v>
+        <v>0.9187783255181492</v>
       </c>
     </row>
     <row r="195">
@@ -5149,7 +5293,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>SUS</t>
+          <t>Não SUS</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
@@ -5159,11 +5303,11 @@
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>01/01/2016</t>
+          <t>01/01/2024</t>
         </is>
       </c>
       <c r="E195" t="n">
-        <v>10.45982087780247</v>
+        <v>27.64687506786431</v>
       </c>
     </row>
     <row r="196">
@@ -5174,7 +5318,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>SUS</t>
+          <t>Não SUS</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
@@ -5184,11 +5328,11 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>01/01/2016</t>
+          <t>01/01/2024</t>
         </is>
       </c>
       <c r="E196" t="n">
-        <v>39.82777949624787</v>
+        <v>7.934903720384016</v>
       </c>
     </row>
     <row r="197">
@@ -5209,11 +5353,11 @@
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>01/01/2017</t>
+          <t>01/01/2012</t>
         </is>
       </c>
       <c r="E197" t="n">
-        <v>54.35779389757344</v>
+        <v>17.8875998975993</v>
       </c>
     </row>
     <row r="198">
@@ -5234,11 +5378,11 @@
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>01/01/2017</t>
+          <t>01/01/2012</t>
         </is>
       </c>
       <c r="E198" t="n">
-        <v>10.41082442211064</v>
+        <v>15.75038016957445</v>
       </c>
     </row>
     <row r="199">
@@ -5259,11 +5403,11 @@
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>01/01/2017</t>
+          <t>01/01/2012</t>
         </is>
       </c>
       <c r="E199" t="n">
-        <v>41.06737974168751</v>
+        <v>99.42717865159091</v>
       </c>
     </row>
     <row r="200">
@@ -5284,11 +5428,11 @@
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>01/01/2018</t>
+          <t>01/01/2013</t>
         </is>
       </c>
       <c r="E200" t="n">
-        <v>49.64210282367441</v>
+        <v>14.58388540470512</v>
       </c>
     </row>
     <row r="201">
@@ -5309,11 +5453,11 @@
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>01/01/2018</t>
+          <t>01/01/2013</t>
         </is>
       </c>
       <c r="E201" t="n">
-        <v>13.21155875325022</v>
+        <v>12.83565939404646</v>
       </c>
     </row>
     <row r="202">
@@ -5334,11 +5478,11 @@
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>01/01/2018</t>
+          <t>01/01/2013</t>
         </is>
       </c>
       <c r="E202" t="n">
-        <v>39.54689181620746</v>
+        <v>96.9805376439066</v>
       </c>
     </row>
     <row r="203">
@@ -5359,11 +5503,11 @@
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>01/01/2019</t>
+          <t>01/01/2014</t>
         </is>
       </c>
       <c r="E203" t="n">
-        <v>47.93592767329795</v>
+        <v>46.33225741054162</v>
       </c>
     </row>
     <row r="204">
@@ -5384,11 +5528,11 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>01/01/2019</t>
+          <t>01/01/2014</t>
         </is>
       </c>
       <c r="E204" t="n">
-        <v>13.04970807803029</v>
+        <v>18.04087899171532</v>
       </c>
     </row>
     <row r="205">
@@ -5409,11 +5553,11 @@
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>01/01/2019</t>
+          <t>01/01/2014</t>
         </is>
       </c>
       <c r="E205" t="n">
-        <v>39.8016096379924</v>
+        <v>55.7171591082521</v>
       </c>
     </row>
     <row r="206">
@@ -5434,11 +5578,11 @@
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
+          <t>01/01/2015</t>
         </is>
       </c>
       <c r="E206" t="n">
-        <v>53.64307176442585</v>
+        <v>54.76715612744778</v>
       </c>
     </row>
     <row r="207">
@@ -5459,11 +5603,11 @@
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
+          <t>01/01/2015</t>
         </is>
       </c>
       <c r="E207" t="n">
-        <v>14.57504682988419</v>
+        <v>10.64666297040995</v>
       </c>
     </row>
     <row r="208">
@@ -5484,11 +5628,11 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
+          <t>01/01/2015</t>
         </is>
       </c>
       <c r="E208" t="n">
-        <v>37.0413172392619</v>
+        <v>43.39868549802699</v>
       </c>
     </row>
     <row r="209">
@@ -5509,11 +5653,11 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
+          <t>01/01/2016</t>
         </is>
       </c>
       <c r="E209" t="n">
-        <v>55.71499917902687</v>
+        <v>55.02580983151642</v>
       </c>
     </row>
     <row r="210">
@@ -5534,11 +5678,11 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
+          <t>01/01/2016</t>
         </is>
       </c>
       <c r="E210" t="n">
-        <v>13.59736741284002</v>
+        <v>10.45982087780247</v>
       </c>
     </row>
     <row r="211">
@@ -5559,11 +5703,11 @@
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
+          <t>01/01/2016</t>
         </is>
       </c>
       <c r="E211" t="n">
-        <v>34.6775628044442</v>
+        <v>39.82777949624787</v>
       </c>
     </row>
     <row r="212">
@@ -5584,11 +5728,11 @@
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
+          <t>01/01/2017</t>
         </is>
       </c>
       <c r="E212" t="n">
-        <v>51.57262579309877</v>
+        <v>54.35779389757344</v>
       </c>
     </row>
     <row r="213">
@@ -5609,11 +5753,11 @@
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
+          <t>01/01/2017</t>
         </is>
       </c>
       <c r="E213" t="n">
-        <v>13.4020968343908</v>
+        <v>10.41082442211064</v>
       </c>
     </row>
     <row r="214">
@@ -5634,11 +5778,11 @@
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
+          <t>01/01/2017</t>
         </is>
       </c>
       <c r="E214" t="n">
-        <v>31.97842092762868</v>
+        <v>41.06737974168751</v>
       </c>
     </row>
     <row r="215">
@@ -5659,11 +5803,11 @@
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>01/01/2023</t>
+          <t>01/01/2018</t>
         </is>
       </c>
       <c r="E215" t="n">
-        <v>54.24063738850477</v>
+        <v>49.64210282367441</v>
       </c>
     </row>
     <row r="216">
@@ -5684,11 +5828,11 @@
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>01/01/2023</t>
+          <t>01/01/2018</t>
         </is>
       </c>
       <c r="E216" t="n">
-        <v>15.6957003459366</v>
+        <v>13.21155875325022</v>
       </c>
     </row>
     <row r="217">
@@ -5709,11 +5853,461 @@
       </c>
       <c r="D217" t="inlineStr">
         <is>
+          <t>01/01/2018</t>
+        </is>
+      </c>
+      <c r="E217" t="n">
+        <v>39.54689181620746</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>SUS</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>Administração Pública</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="E218" t="n">
+        <v>47.93592767329795</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>SUS</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>Entidades Empresariais</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="E219" t="n">
+        <v>13.04970807803029</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>SUS</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>Entidades sem Fins Lucrativos</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="E220" t="n">
+        <v>39.8016096379924</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>SUS</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>Administração Pública</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+      <c r="E221" t="n">
+        <v>53.64307176442585</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>SUS</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>Entidades Empresariais</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+      <c r="E222" t="n">
+        <v>14.57504682988419</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>SUS</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>Entidades sem Fins Lucrativos</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+      <c r="E223" t="n">
+        <v>37.0413172392619</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>SUS</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>Administração Pública</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>01/01/2021</t>
+        </is>
+      </c>
+      <c r="E224" t="n">
+        <v>55.71499917902687</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>SUS</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>Entidades Empresariais</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>01/01/2021</t>
+        </is>
+      </c>
+      <c r="E225" t="n">
+        <v>13.59736741284002</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>SUS</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>Entidades sem Fins Lucrativos</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>01/01/2021</t>
+        </is>
+      </c>
+      <c r="E226" t="n">
+        <v>34.6775628044442</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>SUS</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>Administração Pública</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>01/01/2022</t>
+        </is>
+      </c>
+      <c r="E227" t="n">
+        <v>51.57262579309877</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>SUS</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>Entidades Empresariais</t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>01/01/2022</t>
+        </is>
+      </c>
+      <c r="E228" t="n">
+        <v>13.4020968343908</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>SUS</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>Entidades sem Fins Lucrativos</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>01/01/2022</t>
+        </is>
+      </c>
+      <c r="E229" t="n">
+        <v>31.97842092762868</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>SUS</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>Administração Pública</t>
+        </is>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
           <t>01/01/2023</t>
         </is>
       </c>
-      <c r="E217" t="n">
+      <c r="E230" t="n">
+        <v>54.24063738850477</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>SUS</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>Entidades Empresariais</t>
+        </is>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="E231" t="n">
+        <v>15.6957003459366</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>SUS</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>Entidades sem Fins Lucrativos</t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="E232" t="n">
         <v>30.88644518476532</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>SUS</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>Administração Pública</t>
+        </is>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="E233" t="n">
+        <v>54.83436097296954</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>SUS</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>Entidades Empresariais</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="E234" t="n">
+        <v>15.49394358032879</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>SUS</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>Entidades sem Fins Lucrativos</t>
+        </is>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="E235" t="n">
+        <v>31.23846306761708</v>
       </c>
     </row>
   </sheetData>

</xml_diff>